<commit_message>
added: report and log
</commit_message>
<xml_diff>
--- a/TestData/OrangeHRM.xlsx
+++ b/TestData/OrangeHRM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>admin</t>
   </si>
@@ -48,13 +48,16 @@
   </si>
   <si>
     <t>InvalidLogin</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/auth/login</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +69,14 @@
       <sz val="9.8000000000000007"/>
       <color rgb="FF6AAB73"/>
       <name val="JetBrains Mono"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,16 +96,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -373,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -430,17 +446,31 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>2</v>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C8" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>